<commit_message>
Acronym and glossary works. Install perl.exe(x86), Download xindy package,http://tex.stackexchange.com/questions/156270/has-anyone-managed-to-use-glossaries-with-texstudio-on-windows
</commit_message>
<xml_diff>
--- a/1-Timeline/Sandipan-Timeplan.xlsx
+++ b/1-Timeline/Sandipan-Timeplan.xlsx
@@ -3077,10 +3077,10 @@
   <dimension ref="A1:IV54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="11" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="11" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -3216,12 +3216,12 @@
       <c r="E6" s="31"/>
       <c r="F6" s="97">
         <f ca="1">TODAY()</f>
-        <v>42401</v>
+        <v>42405</v>
       </c>
       <c r="G6" s="97"/>
       <c r="H6" s="5" t="str">
         <f ca="1">TEXT(F6,"dddd")</f>
-        <v>Monday</v>
+        <v>Friday</v>
       </c>
       <c r="I6" s="51"/>
       <c r="J6" s="43"/>
@@ -7646,15 +7646,15 @@
       </c>
       <c r="L16" s="77">
         <f t="shared" ref="L16:L17" ca="1" si="20">ROUNDDOWN(N16*J16,0)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="M16" s="76">
         <f t="shared" ref="M16:M17" ca="1" si="21">J16-L16</f>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="N16" s="78">
         <f>SUMPRODUCT(J17:J24,N17:N24)/SUM(J17:J24)</f>
-        <v>0.4238095238095238</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="O16" s="79"/>
       <c r="P16" s="71"/>
@@ -7930,14 +7930,14 @@
       </c>
       <c r="L17" s="64">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M17" s="63">
         <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="65">
         <v>1</v>
-      </c>
-      <c r="N17" s="65">
-        <v>0.9</v>
       </c>
       <c r="O17" s="66"/>
       <c r="P17" s="58"/>
@@ -8503,7 +8503,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="65">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="O19" s="66"/>
       <c r="P19" s="58"/>
@@ -8779,14 +8779,14 @@
       </c>
       <c r="L20" s="64">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="63">
         <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="65">
         <v>1</v>
-      </c>
-      <c r="N20" s="65">
-        <v>0.8</v>
       </c>
       <c r="O20" s="66"/>
       <c r="P20" s="58"/>
@@ -9051,7 +9051,7 @@
       </c>
       <c r="I21" s="61" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>V</v>
+        <v/>
       </c>
       <c r="J21" s="62">
         <v>2</v>
@@ -9062,14 +9062,14 @@
       </c>
       <c r="L21" s="64">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M21" s="63">
         <f t="shared" si="27"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N21" s="65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="66"/>
       <c r="P21" s="58"/>
@@ -9334,7 +9334,7 @@
       </c>
       <c r="I22" s="61" t="str">
         <f t="shared" ref="I22:I24" ca="1" si="29">IF(AND($F$6&lt;=H22,$F$6&gt;=G22),"V","")</f>
-        <v/>
+        <v>V</v>
       </c>
       <c r="J22" s="62">
         <v>3</v>
@@ -9345,14 +9345,14 @@
       </c>
       <c r="L22" s="64">
         <f t="shared" ref="L22:L24" si="31">ROUNDDOWN(N22*J22,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M22" s="63">
         <f t="shared" ref="M22:M24" si="32">J22-L22</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N22" s="65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="66"/>
       <c r="P22" s="58"/>
@@ -9635,7 +9635,7 @@
         <v>1</v>
       </c>
       <c r="N23" s="65">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="O23" s="66"/>
       <c r="P23" s="58"/>

</xml_diff>